<commit_message>
Documentation - Compiled Final Report
</commit_message>
<xml_diff>
--- a/Team Info/TeamInfo.xlsx
+++ b/Team Info/TeamInfo.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22416"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="15180" windowHeight="6030"/>
+    <workbookView xWindow="80" yWindow="60" windowWidth="24540" windowHeight="14980"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>CSC207 Lab Team Info</t>
   </si>
@@ -125,13 +130,16 @@
   </si>
   <si>
     <t>hjkhok1@e.ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>http://twocube.elasticbeanstalk.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,15 +229,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -526,19 +534,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B6" sqref="B6:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -550,37 +558,39 @@
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+      <c r="B5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:4" ht="74.25" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1"/>
@@ -601,7 +611,7 @@
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="1">
@@ -615,7 +625,7 @@
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="1">
@@ -629,7 +639,7 @@
       <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="1">
@@ -643,7 +653,7 @@
       <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="1">
@@ -657,7 +667,7 @@
       <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="1">
@@ -671,7 +681,7 @@
       <c r="B14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D14" s="1">
@@ -685,7 +695,7 @@
       <c r="B15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D15" s="1">
@@ -699,7 +709,7 @@
       <c r="B16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D16" s="1">
@@ -713,7 +723,7 @@
       <c r="B17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>36</v>
       </c>
       <c r="D17" s="1">
@@ -740,5 +750,10 @@
     <hyperlink ref="C17" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>